<commit_message>
Add one output row as total commissioned spend at 26/27 prices before applying discounted inflation
</commit_message>
<xml_diff>
--- a/DRM2/Model_inputs.xlsx
+++ b/DRM2/Model_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jin.tong\Documents\Rprojects\Dental_Reform_Modelling_2\DRM2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC50593-8E1E-4075-A25D-6128A4916E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C56C3EE-CA8D-45C1-A9D8-DAA95DCF08AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13230" xr2:uid="{2D6CAA86-23AB-4FD8-B2E4-E0C7C9BB22FE}"/>
   </bookViews>
@@ -1394,7 +1394,7 @@
   <dimension ref="A1:X14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="C2" s="87">
         <f>HLOOKUP($C$14, D1:K2, 2,FALSE)</f>
-        <v>6840730</v>
+        <v>79906424</v>
       </c>
       <c r="D2" s="93">
         <v>79906424</v>
@@ -1516,7 +1516,7 @@
       </c>
       <c r="C3" s="88">
         <f>HLOOKUP($C$14, $D$1:K3, 3,FALSE)</f>
-        <v>36.36</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="D3" s="95">
         <v>36.700000000000003</v>
@@ -1564,7 +1564,7 @@
       </c>
       <c r="C4" s="88">
         <f>HLOOKUP($C$14, $D$1:K4, 4,FALSE)</f>
-        <v>4987573</v>
+        <v>71116717.359999999</v>
       </c>
       <c r="D4" s="97">
         <f>D2*D5</f>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="C5" s="88">
         <f>HLOOKUP($C$14, $D$1:K5, 5,FALSE)</f>
-        <v>0.72909999999999997</v>
+        <v>0.89</v>
       </c>
       <c r="D5" s="98">
         <v>0.89</v>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="C7" s="88">
         <f>HLOOKUP($C$14, $D$1:K7, 7,FALSE)</f>
-        <v>0.69</v>
+        <v>0.73</v>
       </c>
       <c r="D7" s="98">
         <v>0.73</v>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="C8" s="88">
         <f>HLOOKUP($C$14, $D$1:K8, 8,FALSE)</f>
-        <v>6634186</v>
+        <v>77493790.564527199</v>
       </c>
       <c r="D8" s="97">
         <v>77493790.564527199</v>
@@ -1901,7 +1901,7 @@
         <v>88</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="24"/>
@@ -1919,7 +1919,7 @@
         <v>105</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="24"/>
@@ -6688,16 +6688,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3cae1bba-4e65-48a6-a71a-8e3da6106e23">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="9dda9b5d-bec3-4bb1-aa3e-36b953cbc3a4" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6953,22 +6949,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3cae1bba-4e65-48a6-a71a-8e3da6106e23">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="9dda9b5d-bec3-4bb1-aa3e-36b953cbc3a4" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F766752A-83BD-4217-AD9D-94A049873B31}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F50563E-D3BD-4B1F-8F16-B11C9744F5E5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3cae1bba-4e65-48a6-a71a-8e3da6106e23"/>
-    <ds:schemaRef ds:uri="9dda9b5d-bec3-4bb1-aa3e-36b953cbc3a4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6994,9 +6990,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F50563E-D3BD-4B1F-8F16-B11C9744F5E5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F766752A-83BD-4217-AD9D-94A049873B31}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3cae1bba-4e65-48a6-a71a-8e3da6106e23"/>
+    <ds:schemaRef ds:uri="9dda9b5d-bec3-4bb1-aa3e-36b953cbc3a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Minor changes to yr0 post-change total spend and PCR calculations; updated ReadMe file
</commit_message>
<xml_diff>
--- a/DRM2/Model_inputs.xlsx
+++ b/DRM2/Model_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jin.tong\Documents\Rprojects\Dental_Reform_Modelling_2\DRM2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C56C3EE-CA8D-45C1-A9D8-DAA95DCF08AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62066EE1-D340-4564-8714-48E18CE978FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13230" xr2:uid="{2D6CAA86-23AB-4FD8-B2E4-E0C7C9BB22FE}"/>
   </bookViews>
@@ -402,7 +402,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
@@ -412,6 +412,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="##,##0"/>
     <numFmt numFmtId="168" formatCode="##,##0.00"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -842,14 +843,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1041,6 +1043,10 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1054,7 +1060,8 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="Comma" xfId="5" builtinId="3"/>
     <cellStyle name="Comma 8" xfId="4" xr:uid="{45A0D5CC-CEB6-4B9A-BCE8-2B756B047F9E}"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1394,7 +1401,7 @@
   <dimension ref="A1:X14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,7 +1472,7 @@
       </c>
       <c r="C2" s="87">
         <f>HLOOKUP($C$14, D1:K2, 2,FALSE)</f>
-        <v>79906424</v>
+        <v>6840730</v>
       </c>
       <c r="D2" s="93">
         <v>79906424</v>
@@ -1516,31 +1523,31 @@
       </c>
       <c r="C3" s="88">
         <f>HLOOKUP($C$14, $D$1:K3, 3,FALSE)</f>
-        <v>36.700000000000003</v>
+        <v>36.356464595445232</v>
       </c>
       <c r="D3" s="95">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="E3" s="60">
-        <v>35.36</v>
+        <v>35.357614315609389</v>
       </c>
       <c r="F3" s="60">
-        <v>38.26</v>
+        <v>38.261389118920356</v>
       </c>
       <c r="G3" s="60">
-        <v>34.6</v>
+        <v>34.59674669069814</v>
       </c>
       <c r="H3" s="60">
-        <v>38.67</v>
+        <v>38.669432475719425</v>
       </c>
       <c r="I3" s="60">
-        <v>37.75</v>
+        <v>37.749442845846509</v>
       </c>
       <c r="J3" s="60">
-        <v>35.840000000000003</v>
+        <v>35.839428789649212</v>
       </c>
       <c r="K3" s="96">
-        <v>36.36</v>
+        <v>36.356464595445232</v>
       </c>
       <c r="L3" t="s">
         <v>90</v>
@@ -1564,32 +1571,39 @@
       </c>
       <c r="C4" s="88">
         <f>HLOOKUP($C$14, $D$1:K4, 4,FALSE)</f>
-        <v>71116717.359999999</v>
-      </c>
-      <c r="D4" s="97">
+        <v>4987572.5109168328</v>
+      </c>
+      <c r="D4" s="106">
         <f>D2*D5</f>
-        <v>71116717.359999999</v>
-      </c>
-      <c r="E4" s="59">
-        <v>7740247</v>
-      </c>
-      <c r="F4" s="59">
-        <v>11416934</v>
-      </c>
-      <c r="G4" s="59">
-        <v>13963736</v>
-      </c>
-      <c r="H4" s="59">
-        <v>11479853</v>
-      </c>
-      <c r="I4" s="59">
-        <v>10678421</v>
-      </c>
-      <c r="J4" s="59">
-        <v>9838682</v>
-      </c>
-      <c r="K4" s="94">
-        <v>4987573</v>
+        <v>71196623.783999994</v>
+      </c>
+      <c r="E4" s="106">
+        <f t="shared" ref="E4:K4" si="0">E2*E5</f>
+        <v>7729465.5474233003</v>
+      </c>
+      <c r="F4" s="106">
+        <f t="shared" si="0"/>
+        <v>11395202.7637231</v>
+      </c>
+      <c r="G4" s="106">
+        <f t="shared" si="0"/>
+        <v>13882922.877151363</v>
+      </c>
+      <c r="H4" s="106">
+        <f t="shared" si="0"/>
+        <v>11460696.035016203</v>
+      </c>
+      <c r="I4" s="106">
+        <f t="shared" si="0"/>
+        <v>10655602.354408357</v>
+      </c>
+      <c r="J4" s="106">
+        <f t="shared" si="0"/>
+        <v>9805453.0896568112</v>
+      </c>
+      <c r="K4" s="106">
+        <f t="shared" si="0"/>
+        <v>4987572.5109168328</v>
       </c>
       <c r="L4" t="s">
         <v>89</v>
@@ -1613,31 +1627,31 @@
       </c>
       <c r="C5" s="88">
         <f>HLOOKUP($C$14, $D$1:K5, 5,FALSE)</f>
-        <v>0.89</v>
-      </c>
-      <c r="D5" s="98">
-        <v>0.89</v>
+        <v>0.72909945443203183</v>
+      </c>
+      <c r="D5" s="107">
+        <v>0.89100000000000001</v>
       </c>
       <c r="E5" s="84">
-        <v>0.87819999999999998</v>
+        <v>0.87693778330688543</v>
       </c>
       <c r="F5" s="84">
-        <v>0.96619999999999995</v>
+        <v>0.96432703092359395</v>
       </c>
       <c r="G5" s="84">
-        <v>0.87929999999999997</v>
+        <v>0.87423887031006231</v>
       </c>
       <c r="H5" s="84">
-        <v>0.85719999999999996</v>
+        <v>0.85576181958681041</v>
       </c>
       <c r="I5" s="84">
-        <v>0.9002</v>
+        <v>0.89827948564569471</v>
       </c>
       <c r="J5" s="84">
-        <v>0.87070000000000003</v>
+        <v>0.86772677149732991</v>
       </c>
       <c r="K5" s="99">
-        <v>0.72909999999999997</v>
+        <v>0.72909945443203183</v>
       </c>
       <c r="L5" t="s">
         <v>89</v>
@@ -1697,31 +1711,31 @@
       </c>
       <c r="C7" s="88">
         <f>HLOOKUP($C$14, $D$1:K7, 7,FALSE)</f>
-        <v>0.73</v>
+        <v>0.69145381562128583</v>
       </c>
       <c r="D7" s="98">
-        <v>0.73</v>
+        <v>0.73000215782769395</v>
       </c>
       <c r="E7" s="83">
-        <v>0.76</v>
+        <v>0.75758755360424745</v>
       </c>
       <c r="F7" s="83">
-        <v>0.83</v>
+        <v>0.83008638928067702</v>
       </c>
       <c r="G7" s="83">
-        <v>0.77</v>
+        <v>0.76568397546477152</v>
       </c>
       <c r="H7" s="83">
-        <v>0.62</v>
+        <v>0.61631321718089616</v>
       </c>
       <c r="I7" s="83">
-        <v>0.48</v>
+        <v>0.47847479498813639</v>
       </c>
       <c r="J7" s="83">
-        <v>0.75</v>
+        <v>0.751447645420808</v>
       </c>
       <c r="K7" s="101">
-        <v>0.69</v>
+        <v>0.69145381562128583</v>
       </c>
       <c r="L7" t="s">
         <v>91</v>
@@ -1739,7 +1753,7 @@
       </c>
       <c r="C8" s="88">
         <f>HLOOKUP($C$14, $D$1:K8, 8,FALSE)</f>
-        <v>77493790.564527199</v>
+        <v>6634186</v>
       </c>
       <c r="D8" s="97">
         <v>77493790.564527199</v>
@@ -1901,7 +1915,7 @@
         <v>88</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="24"/>
@@ -1919,7 +1933,7 @@
         <v>105</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="24"/>
@@ -1954,8 +1968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41FE7DA-E125-467A-80AE-B0E72F949E86}">
   <dimension ref="A1:Y162"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="J155" sqref="J155"/>
+    <sheetView topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="E154" sqref="E154:E162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1970,31 +1984,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="109" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="109" t="s">
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="111" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-      <c r="G1" s="109"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
     </row>
     <row r="2" spans="1:25" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="108" t="s">
+      <c r="B2" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="108"/>
-      <c r="D2" s="106" t="s">
+      <c r="C2" s="110"/>
+      <c r="D2" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
       <c r="G2" s="44" t="s">
         <v>58</v>
       </c>
@@ -2058,7 +2072,7 @@
         <v>1454518</v>
       </c>
       <c r="E4" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F4" s="60">
         <v>23.49</v>
@@ -2084,7 +2098,7 @@
         <v>1048743</v>
       </c>
       <c r="E5" s="60">
-        <v>179.31</v>
+        <v>179.30876935945406</v>
       </c>
       <c r="F5" s="60">
         <v>61.79</v>
@@ -2110,7 +2124,7 @@
         <v>387887</v>
       </c>
       <c r="E6" s="60">
-        <v>383.73</v>
+        <v>383.73474400294782</v>
       </c>
       <c r="F6" s="60">
         <v>76.02</v>
@@ -2133,10 +2147,10 @@
         <v>14</v>
       </c>
       <c r="D7" s="59">
-        <v>5403747</v>
+        <v>5383909.7867940795</v>
       </c>
       <c r="E7" s="60">
-        <v>179.31</v>
+        <v>179.30876935945406</v>
       </c>
       <c r="F7" s="60">
         <v>61.79</v>
@@ -2159,10 +2173,10 @@
         <v>16</v>
       </c>
       <c r="D8" s="59">
-        <v>288475</v>
+        <v>288474.67457258003</v>
       </c>
       <c r="E8" s="60">
-        <v>110.1</v>
+        <v>110.09881241281053</v>
       </c>
       <c r="F8" s="60">
         <v>45.96</v>
@@ -2185,10 +2199,10 @@
         <v>13</v>
       </c>
       <c r="D9" s="59">
-        <v>10866874</v>
+        <v>10839611.202428667</v>
       </c>
       <c r="E9" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F9" s="60">
         <v>23.49</v>
@@ -2211,10 +2225,10 @@
         <v>17</v>
       </c>
       <c r="D10" s="59">
-        <v>8257383</v>
+        <v>8239111.7975713331</v>
       </c>
       <c r="E10" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F10" s="57">
         <v>0</v>
@@ -2237,10 +2251,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="59">
-        <v>2434768</v>
+        <v>2427992.5386333391</v>
       </c>
       <c r="E11" s="60">
-        <v>143.07</v>
+        <v>143.06520141235922</v>
       </c>
       <c r="F11" s="57">
         <v>0</v>
@@ -2263,10 +2277,10 @@
         <v>19</v>
       </c>
       <c r="D12" s="64">
-        <v>2926820</v>
+        <v>2912626</v>
       </c>
       <c r="E12" s="65">
-        <v>44.04</v>
+        <v>44.039524965124208</v>
       </c>
       <c r="F12" s="65">
         <v>17.989999999999998</v>
@@ -2302,7 +2316,7 @@
         <v>1454518</v>
       </c>
       <c r="E14" s="69">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F14" s="69">
         <v>23.49</v>
@@ -2330,7 +2344,7 @@
         <v>1048743</v>
       </c>
       <c r="E15" s="60">
-        <v>179.31</v>
+        <v>179.30876935945406</v>
       </c>
       <c r="F15" s="60">
         <v>61.79</v>
@@ -2383,10 +2397,10 @@
         <v>Returning band 2 &amp; 3</v>
       </c>
       <c r="D17" s="59">
-        <v>5403747</v>
+        <v>5383909.7867940795</v>
       </c>
       <c r="E17" s="60">
-        <v>179.31</v>
+        <v>179.30876935945406</v>
       </c>
       <c r="F17" s="60">
         <v>61.79</v>
@@ -2411,10 +2425,10 @@
         <v>Perio patients</v>
       </c>
       <c r="D18" s="59">
-        <v>288475</v>
+        <v>288474.67457258003</v>
       </c>
       <c r="E18" s="60">
-        <v>256.89999999999998</v>
+        <v>256.89722896322456</v>
       </c>
       <c r="F18" s="60">
         <v>45.96</v>
@@ -2439,10 +2453,10 @@
         <v>Returning band 1</v>
       </c>
       <c r="D19" s="59">
-        <v>10866874</v>
+        <v>10839611.202428667</v>
       </c>
       <c r="E19" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F19" s="60">
         <v>23.49</v>
@@ -2467,10 +2481,10 @@
         <v>Child band 1</v>
       </c>
       <c r="D20" s="59">
-        <v>8257383</v>
+        <v>8239111.7975713331</v>
       </c>
       <c r="E20" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F20" s="57">
         <v>0</v>
@@ -2495,10 +2509,10 @@
         <v>Child band 2 &amp; 3</v>
       </c>
       <c r="D21" s="59">
-        <v>2434768</v>
+        <v>2427992.5386333391</v>
       </c>
       <c r="E21" s="60">
-        <v>143.07</v>
+        <v>143.06520141235922</v>
       </c>
       <c r="F21" s="57">
         <v>0</v>
@@ -2523,7 +2537,7 @@
         <v>Urgent care patients</v>
       </c>
       <c r="D22" s="64">
-        <v>3626820</v>
+        <v>3612626</v>
       </c>
       <c r="E22" s="65">
         <v>75</v>
@@ -2557,7 +2571,7 @@
         <v>194103</v>
       </c>
       <c r="E24" s="69">
-        <v>35.36</v>
+        <v>35.357614315609389</v>
       </c>
       <c r="F24" s="69">
         <v>23.49</v>
@@ -2583,7 +2597,7 @@
         <v>118717</v>
       </c>
       <c r="E25" s="60">
-        <v>172.12</v>
+        <v>172.12694195717168</v>
       </c>
       <c r="F25" s="60">
         <v>61.79</v>
@@ -2609,7 +2623,7 @@
         <v>37987</v>
       </c>
       <c r="E26" s="60">
-        <v>367.7</v>
+        <v>367.70057324312836</v>
       </c>
       <c r="F26" s="60">
         <v>93.01</v>
@@ -2632,10 +2646,10 @@
         <v>14</v>
       </c>
       <c r="D27" s="59">
-        <v>555712</v>
+        <v>554643.05690516951</v>
       </c>
       <c r="E27" s="60">
-        <v>172.12</v>
+        <v>172.12694195717168</v>
       </c>
       <c r="F27" s="60">
         <v>61.79</v>
@@ -2658,10 +2672,10 @@
         <v>16</v>
       </c>
       <c r="D28" s="59">
-        <v>33194</v>
+        <v>33194.381980936079</v>
       </c>
       <c r="E28" s="60">
-        <v>106.07</v>
+        <v>106.07284294682816</v>
       </c>
       <c r="F28" s="60">
         <v>45.96</v>
@@ -2684,10 +2698,10 @@
         <v>13</v>
       </c>
       <c r="D29" s="59">
-        <v>1343248</v>
+        <v>1341014.7366673516</v>
       </c>
       <c r="E29" s="60">
-        <v>35.36</v>
+        <v>35.357614315609389</v>
       </c>
       <c r="F29" s="60">
         <v>23.49</v>
@@ -2710,10 +2724,10 @@
         <v>17</v>
       </c>
       <c r="D30" s="59">
-        <v>1030281</v>
+        <v>1028784.2633326487</v>
       </c>
       <c r="E30" s="60">
-        <v>35.36</v>
+        <v>35.357614315609389</v>
       </c>
       <c r="F30" s="71">
         <v>0</v>
@@ -2736,10 +2750,10 @@
         <v>18</v>
       </c>
       <c r="D31" s="59">
-        <v>254654</v>
+        <v>254288.56111389436</v>
       </c>
       <c r="E31" s="60">
-        <v>137.33000000000001</v>
+        <v>137.33503223275483</v>
       </c>
       <c r="F31" s="71">
         <v>0</v>
@@ -2762,10 +2776,10 @@
         <v>19</v>
       </c>
       <c r="D32" s="64">
-        <v>338230</v>
+        <v>337669</v>
       </c>
       <c r="E32" s="65">
-        <v>42.43</v>
+        <v>42.429137178731267</v>
       </c>
       <c r="F32" s="65">
         <v>17.989999999999998</v>
@@ -2801,7 +2815,7 @@
         <v>194103</v>
       </c>
       <c r="E34" s="69">
-        <v>35.36</v>
+        <v>35.357614315609389</v>
       </c>
       <c r="F34" s="75">
         <v>23.49</v>
@@ -2829,7 +2843,7 @@
         <v>118717</v>
       </c>
       <c r="E35" s="60">
-        <v>172.12</v>
+        <v>172.12694195717168</v>
       </c>
       <c r="F35" s="76">
         <v>61.79</v>
@@ -2882,10 +2896,10 @@
         <v>Returning band 2 &amp; 3</v>
       </c>
       <c r="D37" s="59">
-        <v>555712</v>
+        <v>554643.05690516951</v>
       </c>
       <c r="E37" s="60">
-        <v>172.12</v>
+        <v>172.12694195717168</v>
       </c>
       <c r="F37" s="76">
         <v>61.79</v>
@@ -2910,10 +2924,10 @@
         <v>Perio patients</v>
       </c>
       <c r="D38" s="59">
-        <v>33194</v>
+        <v>33194.381980936079</v>
       </c>
       <c r="E38" s="60">
-        <v>256.89999999999998</v>
+        <v>256.89722896322456</v>
       </c>
       <c r="F38" s="76">
         <v>45.96</v>
@@ -2938,10 +2952,10 @@
         <v>Returning band 1</v>
       </c>
       <c r="D39" s="59">
-        <v>1343248</v>
+        <v>1341014.7366673516</v>
       </c>
       <c r="E39" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F39" s="76">
         <v>23.49</v>
@@ -2966,10 +2980,10 @@
         <v>Child band 1</v>
       </c>
       <c r="D40" s="59">
-        <v>1030281</v>
+        <v>1028784.2633326487</v>
       </c>
       <c r="E40" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F40" s="57">
         <v>0</v>
@@ -2994,10 +3008,10 @@
         <v>Child band 2 &amp; 3</v>
       </c>
       <c r="D41" s="59">
-        <v>254654</v>
+        <v>254288.56111389436</v>
       </c>
       <c r="E41" s="60">
-        <v>137.33000000000001</v>
+        <v>137.33503223275483</v>
       </c>
       <c r="F41" s="57">
         <v>0</v>
@@ -3022,7 +3036,7 @@
         <v>Urgent care patients</v>
       </c>
       <c r="D42" s="77">
-        <v>415444</v>
+        <v>414883.17366894055</v>
       </c>
       <c r="E42" s="65">
         <v>75</v>
@@ -3056,7 +3070,7 @@
         <v>311147</v>
       </c>
       <c r="E44" s="69">
-        <v>38.26</v>
+        <v>38.261389118920356</v>
       </c>
       <c r="F44" s="69">
         <v>23.49</v>
@@ -3082,7 +3096,7 @@
         <v>282495</v>
       </c>
       <c r="E45" s="60">
-        <v>207.63</v>
+        <v>207.66285073088017</v>
       </c>
       <c r="F45" s="60">
         <v>61.79</v>
@@ -3108,7 +3122,7 @@
         <v>57825</v>
       </c>
       <c r="E46" s="60">
-        <v>421.91</v>
+        <v>421.90643549709824</v>
       </c>
       <c r="F46" s="60">
         <v>60.17</v>
@@ -3131,10 +3145,10 @@
         <v>14</v>
       </c>
       <c r="D47" s="59">
-        <v>815420</v>
+        <v>812959.63821323367</v>
       </c>
       <c r="E47" s="60">
-        <v>207.63</v>
+        <v>207.66285073088017</v>
       </c>
       <c r="F47" s="60">
         <v>61.79</v>
@@ -3157,10 +3171,10 @@
         <v>16</v>
       </c>
       <c r="D48" s="59">
-        <v>38012</v>
+        <v>38012.008066009366</v>
       </c>
       <c r="E48" s="60">
-        <v>114.78</v>
+        <v>114.78416735676106</v>
       </c>
       <c r="F48" s="60">
         <v>45.96</v>
@@ -3183,10 +3197,10 @@
         <v>13</v>
       </c>
       <c r="D49" s="59">
-        <v>1098192</v>
+        <v>1095285.3521748993</v>
       </c>
       <c r="E49" s="60">
-        <v>38.26</v>
+        <v>38.261389118920356</v>
       </c>
       <c r="F49" s="60">
         <v>23.49</v>
@@ -3209,10 +3223,10 @@
         <v>17</v>
       </c>
       <c r="D50" s="59">
-        <v>944492</v>
+        <v>942543.64782510081</v>
       </c>
       <c r="E50" s="60">
-        <v>38.26</v>
+        <v>38.261389118920356</v>
       </c>
       <c r="F50" s="71">
         <v>0</v>
@@ -3235,10 +3249,10 @@
         <v>18</v>
       </c>
       <c r="D51" s="59">
-        <v>407710</v>
+        <v>406870.35372075689</v>
       </c>
       <c r="E51" s="60">
-        <v>165.66</v>
+        <v>165.68809028029631</v>
       </c>
       <c r="F51" s="71">
         <v>0</v>
@@ -3261,10 +3275,10 @@
         <v>19</v>
       </c>
       <c r="D52" s="64">
-        <v>490147</v>
+        <v>489233</v>
       </c>
       <c r="E52" s="65">
-        <v>45.91</v>
+        <v>45.913666942704424</v>
       </c>
       <c r="F52" s="65">
         <v>17.989999999999998</v>
@@ -3300,7 +3314,7 @@
         <v>311147</v>
       </c>
       <c r="E54" s="69">
-        <v>38.26</v>
+        <v>38.261389118920356</v>
       </c>
       <c r="F54" s="69">
         <v>23.49</v>
@@ -3328,7 +3342,7 @@
         <v>282495</v>
       </c>
       <c r="E55" s="60">
-        <v>207.63</v>
+        <v>207.66285073088017</v>
       </c>
       <c r="F55" s="60">
         <v>61.79</v>
@@ -3381,10 +3395,10 @@
         <v>Returning band 2 &amp; 3</v>
       </c>
       <c r="D57" s="59">
-        <v>815420</v>
+        <v>812959.63821323367</v>
       </c>
       <c r="E57" s="60">
-        <v>207.63</v>
+        <v>207.66285073088017</v>
       </c>
       <c r="F57" s="60">
         <v>61.79</v>
@@ -3409,10 +3423,10 @@
         <v>Perio patients</v>
       </c>
       <c r="D58" s="59">
-        <v>38012</v>
+        <v>38012.008066009366</v>
       </c>
       <c r="E58" s="60">
-        <v>256.89999999999998</v>
+        <v>256.89722896322456</v>
       </c>
       <c r="F58" s="60">
         <v>45.96</v>
@@ -3437,10 +3451,10 @@
         <v>Returning band 1</v>
       </c>
       <c r="D59" s="59">
-        <v>1098192</v>
+        <v>1095285.3521748993</v>
       </c>
       <c r="E59" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F59" s="60">
         <v>23.49</v>
@@ -3465,10 +3479,10 @@
         <v>Child band 1</v>
       </c>
       <c r="D60" s="59">
-        <v>944492</v>
+        <v>942543.64782510081</v>
       </c>
       <c r="E60" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F60" s="71">
         <v>0</v>
@@ -3493,10 +3507,10 @@
         <v>Child band 2 &amp; 3</v>
       </c>
       <c r="D61" s="59">
-        <v>407710</v>
+        <v>406870.35372075689</v>
       </c>
       <c r="E61" s="60">
-        <v>165.66</v>
+        <v>165.68809028029631</v>
       </c>
       <c r="F61" s="71">
         <v>0</v>
@@ -3521,7 +3535,7 @@
         <v>Urgent care patients</v>
       </c>
       <c r="D62" s="64">
-        <v>593665</v>
+        <v>592750.5682495815</v>
       </c>
       <c r="E62" s="65">
         <v>75</v>
@@ -3555,7 +3569,7 @@
         <v>322784</v>
       </c>
       <c r="E64" s="69">
-        <v>34.6</v>
+        <v>34.59674669069814</v>
       </c>
       <c r="F64" s="69">
         <v>23.49</v>
@@ -3581,7 +3595,7 @@
         <v>266762</v>
       </c>
       <c r="E65" s="60">
-        <v>166.97</v>
+        <v>166.8656011300537</v>
       </c>
       <c r="F65" s="60">
         <v>61.79</v>
@@ -3607,7 +3621,7 @@
         <v>81635</v>
       </c>
       <c r="E66" s="60">
-        <v>359.59</v>
+        <v>359.58714679609233</v>
       </c>
       <c r="F66" s="60">
         <v>77.099999999999994</v>
@@ -3630,10 +3644,10 @@
         <v>14</v>
       </c>
       <c r="D67" s="59">
-        <v>1020093</v>
+        <v>1011290.5843589403</v>
       </c>
       <c r="E67" s="60">
-        <v>166.97</v>
+        <v>166.8656011300537</v>
       </c>
       <c r="F67" s="60">
         <v>61.79</v>
@@ -3656,10 +3670,10 @@
         <v>16</v>
       </c>
       <c r="D68" s="59">
-        <v>58874</v>
+        <v>58873.951534574953</v>
       </c>
       <c r="E68" s="60">
-        <v>103.79</v>
+        <v>103.79024007209442</v>
       </c>
       <c r="F68" s="60">
         <v>45.96</v>
@@ -3682,10 +3696,10 @@
         <v>13</v>
       </c>
       <c r="D69" s="59">
-        <v>2214990</v>
+        <v>2203513.4425999173</v>
       </c>
       <c r="E69" s="60">
-        <v>34.6</v>
+        <v>34.59674669069814</v>
       </c>
       <c r="F69" s="60">
         <v>23.49</v>
@@ -3708,10 +3722,10 @@
         <v>17</v>
       </c>
       <c r="D70" s="59">
-        <v>1700730</v>
+        <v>1693039.5574000832</v>
       </c>
       <c r="E70" s="60">
-        <v>34.6</v>
+        <v>34.59674669069814</v>
       </c>
       <c r="F70" s="71">
         <v>0</v>
@@ -3734,10 +3748,10 @@
         <v>18</v>
       </c>
       <c r="D71" s="59">
-        <v>487498</v>
+        <v>484491.46410648461</v>
       </c>
       <c r="E71" s="60">
-        <v>133.22</v>
+        <v>133.13716289362753</v>
       </c>
       <c r="F71" s="71">
         <v>0</v>
@@ -3760,10 +3774,10 @@
         <v>19</v>
       </c>
       <c r="D72" s="64">
-        <v>510157</v>
+        <v>508149</v>
       </c>
       <c r="E72" s="65">
-        <v>41.52</v>
+        <v>41.516096028837765</v>
       </c>
       <c r="F72" s="65">
         <v>17.989999999999998</v>
@@ -3799,7 +3813,7 @@
         <v>322784</v>
       </c>
       <c r="E74" s="69">
-        <v>34.6</v>
+        <v>34.59674669069814</v>
       </c>
       <c r="F74" s="75">
         <v>23.49</v>
@@ -3827,7 +3841,7 @@
         <v>266762</v>
       </c>
       <c r="E75" s="60">
-        <v>166.97</v>
+        <v>166.8656011300537</v>
       </c>
       <c r="F75" s="76">
         <v>61.79</v>
@@ -3880,10 +3894,10 @@
         <v>Returning band 2 &amp; 3</v>
       </c>
       <c r="D77" s="59">
-        <v>1020093</v>
+        <v>1011290.5843589403</v>
       </c>
       <c r="E77" s="60">
-        <v>166.97</v>
+        <v>166.8656011300537</v>
       </c>
       <c r="F77" s="76">
         <v>61.79</v>
@@ -3908,10 +3922,10 @@
         <v>Perio patients</v>
       </c>
       <c r="D78" s="59">
-        <v>58874</v>
+        <v>58873.951534574953</v>
       </c>
       <c r="E78" s="60">
-        <v>256.89999999999998</v>
+        <v>256.89722896322456</v>
       </c>
       <c r="F78" s="76">
         <v>45.96</v>
@@ -3936,10 +3950,10 @@
         <v>Returning band 1</v>
       </c>
       <c r="D79" s="59">
-        <v>2214990</v>
+        <v>2203513.4425999173</v>
       </c>
       <c r="E79" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F79" s="76">
         <v>23.49</v>
@@ -3964,10 +3978,10 @@
         <v>Child band 1</v>
       </c>
       <c r="D80" s="59">
-        <v>1700730</v>
+        <v>1693039.5574000832</v>
       </c>
       <c r="E80" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F80" s="57">
         <v>0</v>
@@ -3992,10 +4006,10 @@
         <v>Child band 2 &amp; 3</v>
       </c>
       <c r="D81" s="59">
-        <v>487498</v>
+        <v>484491.46410648461</v>
       </c>
       <c r="E81" s="60">
-        <v>133.22</v>
+        <v>133.13716289362753</v>
       </c>
       <c r="F81" s="57">
         <v>0</v>
@@ -4020,7 +4034,7 @@
         <v>Urgent care patients</v>
       </c>
       <c r="D82" s="77">
-        <v>649270</v>
+        <v>647261.8165114735</v>
       </c>
       <c r="E82" s="65">
         <v>75</v>
@@ -4054,7 +4068,7 @@
         <v>170846</v>
       </c>
       <c r="E84" s="69">
-        <v>38.67</v>
+        <v>38.669432475719425</v>
       </c>
       <c r="F84" s="69">
         <v>23.49</v>
@@ -4080,7 +4094,7 @@
         <v>115637</v>
       </c>
       <c r="E85" s="60">
-        <v>178.3</v>
+        <v>178.32811346650587</v>
       </c>
       <c r="F85" s="60">
         <v>61.79</v>
@@ -4106,7 +4120,7 @@
         <v>71990</v>
       </c>
       <c r="E86" s="60">
-        <v>397.14</v>
+        <v>397.14038931119291</v>
       </c>
       <c r="F86" s="60">
         <v>63.58</v>
@@ -4129,10 +4143,10 @@
         <v>14</v>
       </c>
       <c r="D87" s="59">
-        <v>975498</v>
+        <v>973265.08127999189</v>
       </c>
       <c r="E87" s="60">
-        <v>178.3</v>
+        <v>178.32811346650587</v>
       </c>
       <c r="F87" s="60">
         <v>61.79</v>
@@ -4155,10 +4169,10 @@
         <v>16</v>
       </c>
       <c r="D88" s="59">
-        <v>50247</v>
+        <v>50246.946787724926</v>
       </c>
       <c r="E88" s="60">
-        <v>116.01</v>
+        <v>116.00829742715828</v>
       </c>
       <c r="F88" s="60">
         <v>45.96</v>
@@ -4181,10 +4195,10 @@
         <v>13</v>
       </c>
       <c r="D89" s="59">
-        <v>1911950</v>
+        <v>1908956.3996125823</v>
       </c>
       <c r="E89" s="60">
-        <v>38.67</v>
+        <v>38.669432475719425</v>
       </c>
       <c r="F89" s="60">
         <v>23.49</v>
@@ -4207,10 +4221,10 @@
         <v>17</v>
       </c>
       <c r="D90" s="59">
-        <v>1395820</v>
+        <v>1393813.6003874179</v>
       </c>
       <c r="E90" s="60">
-        <v>38.67</v>
+        <v>38.669432475719425</v>
       </c>
       <c r="F90" s="71">
         <v>0</v>
@@ -4233,10 +4247,10 @@
         <v>18</v>
       </c>
       <c r="D91" s="59">
-        <v>414412</v>
+        <v>413648.97193228296</v>
       </c>
       <c r="E91" s="60">
-        <v>142.26</v>
+        <v>142.28276487374458</v>
       </c>
       <c r="F91" s="71">
         <v>0</v>
@@ -4259,10 +4273,10 @@
         <v>19</v>
       </c>
       <c r="D92" s="64">
-        <v>462759</v>
+        <v>461167</v>
       </c>
       <c r="E92" s="65">
-        <v>46.4</v>
+        <v>46.40331897086331</v>
       </c>
       <c r="F92" s="65">
         <v>17.989999999999998</v>
@@ -4298,7 +4312,7 @@
         <v>170846</v>
       </c>
       <c r="E94" s="69">
-        <v>38.67</v>
+        <v>38.669432475719425</v>
       </c>
       <c r="F94" s="69">
         <v>23.49</v>
@@ -4326,7 +4340,7 @@
         <v>115637</v>
       </c>
       <c r="E95" s="60">
-        <v>178.3</v>
+        <v>178.32811346650587</v>
       </c>
       <c r="F95" s="60">
         <v>61.79</v>
@@ -4379,10 +4393,10 @@
         <v>Returning band 2 &amp; 3</v>
       </c>
       <c r="D97" s="59">
-        <v>975498</v>
+        <v>973265.08127999189</v>
       </c>
       <c r="E97" s="60">
-        <v>178.3</v>
+        <v>178.32811346650587</v>
       </c>
       <c r="F97" s="60">
         <v>61.79</v>
@@ -4407,10 +4421,10 @@
         <v>Perio patients</v>
       </c>
       <c r="D98" s="59">
-        <v>50247</v>
+        <v>50246.946787724926</v>
       </c>
       <c r="E98" s="60">
-        <v>256.89999999999998</v>
+        <v>256.89722896322456</v>
       </c>
       <c r="F98" s="60">
         <v>45.96</v>
@@ -4435,10 +4449,10 @@
         <v>Returning band 1</v>
       </c>
       <c r="D99" s="59">
-        <v>1911950</v>
+        <v>1908956.3996125823</v>
       </c>
       <c r="E99" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F99" s="60">
         <v>23.49</v>
@@ -4463,10 +4477,10 @@
         <v>Child band 1</v>
       </c>
       <c r="D100" s="59">
-        <v>1395820</v>
+        <v>1393813.6003874179</v>
       </c>
       <c r="E100" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F100" s="71">
         <v>0</v>
@@ -4491,10 +4505,10 @@
         <v>Child band 2 &amp; 3</v>
       </c>
       <c r="D101" s="59">
-        <v>414412</v>
+        <v>413648.97193228296</v>
       </c>
       <c r="E101" s="60">
-        <v>142.26</v>
+        <v>142.28276487374458</v>
       </c>
       <c r="F101" s="71">
         <v>0</v>
@@ -4519,7 +4533,7 @@
         <v>Urgent care patients</v>
       </c>
       <c r="D102" s="64">
-        <v>580080</v>
+        <v>578487.64245548018</v>
       </c>
       <c r="E102" s="65">
         <v>75</v>
@@ -4553,7 +4567,7 @@
         <v>106648</v>
       </c>
       <c r="E104" s="69">
-        <v>37.75</v>
+        <v>37.749442845846509</v>
       </c>
       <c r="F104" s="69">
         <v>23.49</v>
@@ -4579,7 +4593,7 @@
         <v>57472</v>
       </c>
       <c r="E105" s="60">
-        <v>181.45</v>
+        <v>181.47748086328383</v>
       </c>
       <c r="F105" s="60">
         <v>61.79</v>
@@ -4605,7 +4619,7 @@
         <v>62643</v>
       </c>
       <c r="E106" s="60">
-        <v>397.31</v>
+        <v>397.30976743385634</v>
       </c>
       <c r="F106" s="60">
         <v>75.08</v>
@@ -4628,10 +4642,10 @@
         <v>14</v>
       </c>
       <c r="D107" s="59">
-        <v>941253</v>
+        <v>939862.23797267035</v>
       </c>
       <c r="E107" s="60">
-        <v>181.45</v>
+        <v>181.47748086328383</v>
       </c>
       <c r="F107" s="60">
         <v>61.79</v>
@@ -4654,10 +4668,10 @@
         <v>16</v>
       </c>
       <c r="D108" s="59">
-        <v>42701</v>
+        <v>42701.133603267248</v>
       </c>
       <c r="E108" s="60">
-        <v>113.25</v>
+        <v>113.24832853753952</v>
       </c>
       <c r="F108" s="60">
         <v>45.96</v>
@@ -4680,10 +4694,10 @@
         <v>13</v>
       </c>
       <c r="D109" s="59">
-        <v>1723985</v>
+        <v>1720683.1425587691</v>
       </c>
       <c r="E109" s="60">
-        <v>37.75</v>
+        <v>37.749442845846509</v>
       </c>
       <c r="F109" s="60">
         <v>23.49</v>
@@ -4706,10 +4720,10 @@
         <v>17</v>
       </c>
       <c r="D110" s="59">
-        <v>1226828</v>
+        <v>1224615.8574412311</v>
       </c>
       <c r="E110" s="60">
-        <v>37.75</v>
+        <v>37.749442845846509</v>
       </c>
       <c r="F110" s="71">
         <v>0</v>
@@ -4732,10 +4746,10 @@
         <v>18</v>
       </c>
       <c r="D111" s="59">
-        <v>377081</v>
+        <v>376605.62842406222</v>
       </c>
       <c r="E111" s="60">
-        <v>144.77000000000001</v>
+        <v>144.79555263393681</v>
       </c>
       <c r="F111" s="71">
         <v>0</v>
@@ -4758,10 +4772,10 @@
         <v>19</v>
       </c>
       <c r="D112" s="64">
-        <v>489113</v>
+        <v>480906</v>
       </c>
       <c r="E112" s="65">
-        <v>45.3</v>
+        <v>45.299331415015807</v>
       </c>
       <c r="F112" s="65">
         <v>17.989999999999998</v>
@@ -4797,7 +4811,7 @@
         <v>106648</v>
       </c>
       <c r="E114" s="69">
-        <v>37.75</v>
+        <v>37.749442845846509</v>
       </c>
       <c r="F114" s="69">
         <v>23.49</v>
@@ -4825,7 +4839,7 @@
         <v>57472</v>
       </c>
       <c r="E115" s="60">
-        <v>181.45</v>
+        <v>181.47748086328383</v>
       </c>
       <c r="F115" s="60">
         <v>61.79</v>
@@ -4878,10 +4892,10 @@
         <v>Returning band 2 &amp; 3</v>
       </c>
       <c r="D117" s="59">
-        <v>941253</v>
+        <v>939862.23797267035</v>
       </c>
       <c r="E117" s="60">
-        <v>181.45</v>
+        <v>181.47748086328383</v>
       </c>
       <c r="F117" s="60">
         <v>61.79</v>
@@ -4906,10 +4920,10 @@
         <v>Perio patients</v>
       </c>
       <c r="D118" s="59">
-        <v>42701</v>
+        <v>42701.133603267248</v>
       </c>
       <c r="E118" s="60">
-        <v>256.89999999999998</v>
+        <v>256.89722896322456</v>
       </c>
       <c r="F118" s="60">
         <v>45.96</v>
@@ -4934,10 +4948,10 @@
         <v>Returning band 1</v>
       </c>
       <c r="D119" s="59">
-        <v>1723985</v>
+        <v>1720683.1425587691</v>
       </c>
       <c r="E119" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F119" s="60">
         <v>23.49</v>
@@ -4962,10 +4976,10 @@
         <v>Child band 1</v>
       </c>
       <c r="D120" s="59">
-        <v>1226828</v>
+        <v>1224615.8574412311</v>
       </c>
       <c r="E120" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F120" s="71">
         <v>0</v>
@@ -4990,10 +5004,10 @@
         <v>Child band 2 &amp; 3</v>
       </c>
       <c r="D121" s="59">
-        <v>377081</v>
+        <v>376605.62842406222</v>
       </c>
       <c r="E121" s="60">
-        <v>144.77000000000001</v>
+        <v>144.79555263393681</v>
       </c>
       <c r="F121" s="71">
         <v>0</v>
@@ -5018,7 +5032,7 @@
         <v>Urgent care patients</v>
       </c>
       <c r="D122" s="64">
-        <v>593029</v>
+        <v>584822.10692026466</v>
       </c>
       <c r="E122" s="65">
         <v>75</v>
@@ -5052,7 +5066,7 @@
         <v>248695</v>
       </c>
       <c r="E124" s="69">
-        <v>35.840000000000003</v>
+        <v>35.839428789649212</v>
       </c>
       <c r="F124" s="69">
         <v>23.49</v>
@@ -5078,7 +5092,7 @@
         <v>145992</v>
       </c>
       <c r="E125" s="60">
-        <v>176.71</v>
+        <v>176.69378435926555</v>
       </c>
       <c r="F125" s="60">
         <v>61.79</v>
@@ -5104,7 +5118,7 @@
         <v>48289</v>
       </c>
       <c r="E126" s="60">
-        <v>371.08</v>
+        <v>371.07780452258294</v>
       </c>
       <c r="F126" s="60">
         <v>92.96</v>
@@ -5127,10 +5141,10 @@
         <v>14</v>
       </c>
       <c r="D127" s="59">
-        <v>712958</v>
+        <v>709076.2136203578</v>
       </c>
       <c r="E127" s="60">
-        <v>176.71</v>
+        <v>176.69378435926555</v>
       </c>
       <c r="F127" s="60">
         <v>61.79</v>
@@ -5153,10 +5167,10 @@
         <v>16</v>
       </c>
       <c r="D128" s="59">
-        <v>42217</v>
+        <v>42217.047945793951</v>
       </c>
       <c r="E128" s="60">
-        <v>107.52</v>
+        <v>107.51828636894763</v>
       </c>
       <c r="F128" s="60">
         <v>45.96</v>
@@ -5179,10 +5193,10 @@
         <v>13</v>
       </c>
       <c r="D129" s="59">
-        <v>1660157</v>
+        <v>1655805.7007587738</v>
       </c>
       <c r="E129" s="60">
-        <v>35.840000000000003</v>
+        <v>35.839428789649212</v>
       </c>
       <c r="F129" s="60">
         <v>23.49</v>
@@ -5205,10 +5219,10 @@
         <v>17</v>
       </c>
       <c r="D130" s="59">
-        <v>1279249</v>
+        <v>1276332.2992412264</v>
       </c>
       <c r="E130" s="60">
-        <v>35.840000000000003</v>
+        <v>35.839428789649212</v>
       </c>
       <c r="F130" s="71">
         <v>0</v>
@@ -5231,10 +5245,10 @@
         <v>18</v>
       </c>
       <c r="D131" s="59">
-        <v>324274</v>
+        <v>322948.73843384819</v>
       </c>
       <c r="E131" s="60">
-        <v>140.99</v>
+        <v>140.97878167349916</v>
       </c>
       <c r="F131" s="71">
         <v>0</v>
@@ -5257,10 +5271,10 @@
         <v>19</v>
       </c>
       <c r="D132" s="64">
-        <v>427592</v>
+        <v>426680</v>
       </c>
       <c r="E132" s="65">
-        <v>43.01</v>
+        <v>43.00731454757905</v>
       </c>
       <c r="F132" s="65">
         <v>17.989999999999998</v>
@@ -5296,7 +5310,7 @@
         <v>248695</v>
       </c>
       <c r="E134" s="69">
-        <v>35.840000000000003</v>
+        <v>35.839428789649212</v>
       </c>
       <c r="F134" s="69">
         <v>23.49</v>
@@ -5324,7 +5338,7 @@
         <v>145992</v>
       </c>
       <c r="E135" s="60">
-        <v>176.71</v>
+        <v>176.69378435926555</v>
       </c>
       <c r="F135" s="60">
         <v>61.79</v>
@@ -5377,10 +5391,10 @@
         <v>Returning band 2 &amp; 3</v>
       </c>
       <c r="D137" s="59">
-        <v>712958</v>
+        <v>709076.2136203578</v>
       </c>
       <c r="E137" s="60">
-        <v>176.71</v>
+        <v>176.69378435926555</v>
       </c>
       <c r="F137" s="60">
         <v>61.79</v>
@@ -5405,10 +5419,10 @@
         <v>Perio patients</v>
       </c>
       <c r="D138" s="59">
-        <v>42217</v>
+        <v>42217.047945793951</v>
       </c>
       <c r="E138" s="60">
-        <v>256.89999999999998</v>
+        <v>256.89722896322456</v>
       </c>
       <c r="F138" s="60">
         <v>45.96</v>
@@ -5433,10 +5447,10 @@
         <v>Returning band 1</v>
       </c>
       <c r="D139" s="59">
-        <v>1660157</v>
+        <v>1655805.7007587738</v>
       </c>
       <c r="E139" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F139" s="60">
         <v>23.49</v>
@@ -5461,10 +5475,10 @@
         <v>Child band 1</v>
       </c>
       <c r="D140" s="59">
-        <v>1279249</v>
+        <v>1276332.2992412264</v>
       </c>
       <c r="E140" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F140" s="71">
         <v>0</v>
@@ -5489,10 +5503,10 @@
         <v>Child band 2 &amp; 3</v>
       </c>
       <c r="D141" s="59">
-        <v>324274</v>
+        <v>322948.73843384819</v>
       </c>
       <c r="E141" s="60">
-        <v>140.99</v>
+        <v>140.97878167349916</v>
       </c>
       <c r="F141" s="71">
         <v>0</v>
@@ -5517,7 +5531,7 @@
         <v>Urgent care patients</v>
       </c>
       <c r="D142" s="64">
-        <v>526584</v>
+        <v>525672.20868650055</v>
       </c>
       <c r="E142" s="65">
         <v>75</v>
@@ -5551,7 +5565,7 @@
         <v>100295</v>
       </c>
       <c r="E144" s="69">
-        <v>36.36</v>
+        <v>36.356464595445232</v>
       </c>
       <c r="F144" s="69">
         <v>23.49</v>
@@ -5577,7 +5591,7 @@
         <v>61668</v>
       </c>
       <c r="E145" s="60">
-        <v>169.2</v>
+        <v>169.20371166638463</v>
       </c>
       <c r="F145" s="60">
         <v>61.79</v>
@@ -5603,7 +5617,7 @@
         <v>27518</v>
       </c>
       <c r="E146" s="60">
-        <v>364.62</v>
+        <v>364.62291792701348</v>
       </c>
       <c r="F146" s="60">
         <v>87.68</v>
@@ -5626,10 +5640,10 @@
         <v>14</v>
       </c>
       <c r="D147" s="59">
-        <v>382813</v>
+        <v>382812.97444371646</v>
       </c>
       <c r="E147" s="60">
-        <v>169.2</v>
+        <v>169.20371166638463</v>
       </c>
       <c r="F147" s="60">
         <v>61.79</v>
@@ -5652,10 +5666,10 @@
         <v>16</v>
       </c>
       <c r="D148" s="59">
-        <v>23229</v>
+        <v>23229.204654273493</v>
       </c>
       <c r="E148" s="60">
-        <v>109.07</v>
+        <v>109.0693937863357</v>
       </c>
       <c r="F148" s="60">
         <v>45.96</v>
@@ -5678,10 +5692,10 @@
         <v>13</v>
       </c>
       <c r="D149" s="59">
-        <v>914352</v>
+        <v>914352.42805637419</v>
       </c>
       <c r="E149" s="60">
-        <v>36.36</v>
+        <v>36.356464595445232</v>
       </c>
       <c r="F149" s="60">
         <v>23.49</v>
@@ -5704,10 +5718,10 @@
         <v>17</v>
       </c>
       <c r="D150" s="59">
-        <v>679983</v>
+        <v>679982.57194362592</v>
       </c>
       <c r="E150" s="60">
-        <v>36.36</v>
+        <v>36.356464595445232</v>
       </c>
       <c r="F150" s="71">
         <v>0</v>
@@ -5730,10 +5744,10 @@
         <v>18</v>
       </c>
       <c r="D151" s="59">
-        <v>169139</v>
+        <v>169138.82090200999</v>
       </c>
       <c r="E151" s="60">
-        <v>135</v>
+        <v>135.00267262859191</v>
       </c>
       <c r="F151" s="71">
         <v>0</v>
@@ -5759,7 +5773,7 @@
         <v>208822</v>
       </c>
       <c r="E152" s="65">
-        <v>43.63</v>
+        <v>43.627757514534274</v>
       </c>
       <c r="F152" s="65">
         <v>17.989999999999998</v>
@@ -5795,7 +5809,7 @@
         <v>100295</v>
       </c>
       <c r="E154" s="69">
-        <v>36.36</v>
+        <v>36.356464595445232</v>
       </c>
       <c r="F154" s="69">
         <v>23.49</v>
@@ -5823,7 +5837,7 @@
         <v>61668</v>
       </c>
       <c r="E155" s="60">
-        <v>169.2</v>
+        <v>169.20371166638463</v>
       </c>
       <c r="F155" s="60">
         <v>61.79</v>
@@ -5876,10 +5890,10 @@
         <v>Returning band 2 &amp; 3</v>
       </c>
       <c r="D157" s="59">
-        <v>382813</v>
+        <v>382812.97444371646</v>
       </c>
       <c r="E157" s="60">
-        <v>169.2</v>
+        <v>169.20371166638463</v>
       </c>
       <c r="F157" s="60">
         <v>61.79</v>
@@ -5904,10 +5918,10 @@
         <v>Perio patients</v>
       </c>
       <c r="D158" s="59">
-        <v>23229</v>
+        <v>23229.204654273493</v>
       </c>
       <c r="E158" s="60">
-        <v>256.89999999999998</v>
+        <v>256.89722896322456</v>
       </c>
       <c r="F158" s="60">
         <v>45.96</v>
@@ -5932,10 +5946,10 @@
         <v>Returning band 1</v>
       </c>
       <c r="D159" s="59">
-        <v>914352</v>
+        <v>914352.42805637419</v>
       </c>
       <c r="E159" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F159" s="60">
         <v>23.49</v>
@@ -5960,10 +5974,10 @@
         <v>Child band 1</v>
       </c>
       <c r="D160" s="59">
-        <v>679983</v>
+        <v>679982.57194362592</v>
       </c>
       <c r="E160" s="60">
-        <v>36.700000000000003</v>
+        <v>36.699604137603508</v>
       </c>
       <c r="F160" s="71">
         <v>0</v>
@@ -5988,10 +6002,10 @@
         <v>Child band 2 &amp; 3</v>
       </c>
       <c r="D161" s="59">
-        <v>169139</v>
+        <v>169138.82090200999</v>
       </c>
       <c r="E161" s="60">
-        <v>135</v>
+        <v>135.00267262859191</v>
       </c>
       <c r="F161" s="71">
         <v>0</v>
@@ -6016,7 +6030,7 @@
         <v>Urgent care patients</v>
       </c>
       <c r="D162" s="64">
-        <v>268748</v>
+        <v>268748.48350775905</v>
       </c>
       <c r="E162" s="65">
         <v>75</v>
@@ -6688,15 +6702,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B23CEB47A3A02045B6F2DCDFB32E39E0" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4997c10e2bfde837ec4696a9c931eed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3cae1bba-4e65-48a6-a71a-8e3da6106e23" xmlns:ns3="9dda9b5d-bec3-4bb1-aa3e-36b953cbc3a4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="086ee537026ec87015cd255953686a31" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6948,7 +6953,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="3cae1bba-4e65-48a6-a71a-8e3da6106e23">
@@ -6961,15 +6966,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F50563E-D3BD-4B1F-8F16-B11C9744F5E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34F1A255-E3A0-41B6-B096-D5E2D81B675A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6989,7 +6995,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F766752A-83BD-4217-AD9D-94A049873B31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -6999,4 +7005,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F50563E-D3BD-4B1F-8F16-B11C9744F5E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>